<commit_message>
Doc: - Updated the ReadMe - Created Data Models and Mapping sheets
</commit_message>
<xml_diff>
--- a/data_models_and_catalogs/edge_node/edge_node_data_catalog.xlsx
+++ b/data_models_and_catalogs/edge_node/edge_node_data_catalog.xlsx
@@ -5,12 +5,11 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="source files" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="Flights" sheetId="2" state="visible" r:id="rId3"/>
-    <sheet name="Basic Model" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="Flights Atts. Description" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -22,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="425" uniqueCount="349">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="417" uniqueCount="346">
   <si>
     <t xml:space="preserve">Source File</t>
   </si>
@@ -33,13 +32,13 @@
     <t xml:space="preserve">Flights.zip</t>
   </si>
   <si>
-    <t xml:space="preserve">Transaction</t>
+    <t xml:space="preserve">gzip</t>
   </si>
   <si>
     <t xml:space="preserve">L_AIRLINE_ID.csv</t>
   </si>
   <si>
-    <t xml:space="preserve">Lookup</t>
+    <t xml:space="preserve">csv</t>
   </si>
   <si>
     <t xml:space="preserve">L_AIRPORT_ID.csv</t>
@@ -96,6 +95,12 @@
     <t xml:space="preserve">L_YESNO_RESP.csv</t>
   </si>
   <si>
+    <t xml:space="preserve">us-cities-demographics.json</t>
+  </si>
+  <si>
+    <t xml:space="preserve">json</t>
+  </si>
+  <si>
     <t xml:space="preserve">Logical Col Name</t>
   </si>
   <si>
@@ -1054,21 +1059,6 @@
   </si>
   <si>
     <t xml:space="preserve">Aircraft Tail Number for Diverted Airport Code5 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Flight</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CALENDAR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AIRLINE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DATE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">L_AIRLINE_ID.CODE</t>
   </si>
 </sst>
 </file>
@@ -1139,7 +1129,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1150,12 +1140,6 @@
       <patternFill patternType="solid">
         <fgColor rgb="FF00599D"/>
         <bgColor rgb="FF008080"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFF200"/>
-        <bgColor rgb="FFFFFF00"/>
       </patternFill>
     </fill>
   </fills>
@@ -1221,7 +1205,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="15">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1282,18 +1266,6 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
@@ -1310,7 +1282,7 @@
       <rgbColor rgb="FFFF0000"/>
       <rgbColor rgb="FF00FF00"/>
       <rgbColor rgb="FF0000FF"/>
-      <rgbColor rgb="FFFFF200"/>
+      <rgbColor rgb="FFFFFF00"/>
       <rgbColor rgb="FFFF00FF"/>
       <rgbColor rgb="FF00FFFF"/>
       <rgbColor rgb="FF800000"/>
@@ -1371,10 +1343,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AMJ21"/>
+  <dimension ref="A1:AMJ22"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B17" activeCellId="0" sqref="B17"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B22" activeCellId="0" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1552,6 +1524,14 @@
       </c>
       <c r="B21" s="5" t="s">
         <v>5</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -1572,7 +1552,7 @@
   </sheetPr>
   <dimension ref="A1:D110"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A58" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C14" activeCellId="0" sqref="C14"/>
     </sheetView>
   </sheetViews>
@@ -1587,1245 +1567,1245 @@
   <sheetData>
     <row r="1" s="9" customFormat="true" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="3" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="D1" s="8" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="10" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B2" s="11" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C2" s="12" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D2" s="13"/>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="10" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B3" s="11" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C3" s="12" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="D3" s="11" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="10" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="D4" s="13" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="10" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C5" s="12" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="D5" s="13"/>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="10" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B6" s="11" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="D6" s="13" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="10" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="B7" s="11" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="C7" s="12" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="D7" s="13"/>
     </row>
     <row r="8" customFormat="false" ht="55.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="10" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="B8" s="11" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="C8" s="12" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="D8" s="13" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="69" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="10" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="C9" s="12" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="D9" s="13" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="69" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="10" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="B10" s="11" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="C10" s="12" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="D10" s="13" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="11" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="B11" s="11" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="C11" s="12" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="D11" s="13"/>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="10" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="B12" s="11" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="C12" s="14" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="D12" s="13"/>
     </row>
     <row r="13" customFormat="false" ht="82.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="10" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="B13" s="11" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="C13" s="14" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="D13" s="11" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="69" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="10" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="B14" s="11" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="C14" s="14" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="D14" s="13" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="69" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="10" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="B15" s="11" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="C15" s="14" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="D15" s="13" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="10" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="B16" s="11" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="C16" s="12" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="D16" s="11" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="10" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="B17" s="11" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="C17" s="14" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="D17" s="13"/>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="10" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="B18" s="11" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="C18" s="14" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="D18" s="13" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="10" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="B19" s="11" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="C19" s="14" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="D19" s="13" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="10" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="B20" s="11" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="C20" s="12" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="D20" s="13"/>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="10" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="B21" s="11" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="C21" s="14" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="D21" s="11" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="82.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="10" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="B22" s="11" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="C22" s="14" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="D22" s="11" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="69" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="10" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="B23" s="11" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="C23" s="14" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="D23" s="13" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="69" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="10" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="B24" s="11" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="C24" s="14" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="D24" s="13" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="10" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="B25" s="11" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="C25" s="14" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="D25" s="11" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="10" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="B26" s="11" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="C26" s="14" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="D26" s="13"/>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="10" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="B27" s="11" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="C27" s="14" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="D27" s="13" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="10" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="B28" s="11" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="C28" s="14" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="D28" s="13" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="10" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="B29" s="11" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="C29" s="14" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="D29" s="13"/>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="10" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="B30" s="11" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="C30" s="14" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="D30" s="11" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="10" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="B31" s="11" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="C31" s="14" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="D31" s="13"/>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="10" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="B32" s="11" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="C32" s="14" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="D32" s="13"/>
     </row>
     <row r="33" customFormat="false" ht="42" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="10" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="B33" s="11" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="C33" s="14" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="D33" s="13"/>
     </row>
     <row r="34" customFormat="false" ht="42" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="10" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="B34" s="11" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="C34" s="14" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="D34" s="13"/>
     </row>
     <row r="35" customFormat="false" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="10" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="B35" s="11" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="C35" s="14" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="D35" s="11" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="10" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="B36" s="11" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="C36" s="14" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="D36" s="11" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="10" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="B37" s="11" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="C37" s="14" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="D37" s="11" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="10" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="B38" s="11" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="C38" s="14" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="D38" s="13"/>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="10" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="B39" s="11" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="C39" s="14" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="D39" s="13"/>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="10" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="B40" s="11" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="C40" s="14" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="D40" s="13"/>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="10" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="B41" s="11" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="C41" s="14" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="D41" s="13"/>
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="10" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="B42" s="11" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="C42" s="14" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="D42" s="13"/>
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="10" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="B43" s="11" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="C43" s="14" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="D43" s="13"/>
     </row>
     <row r="44" customFormat="false" ht="42" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="11" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="B44" s="11" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="C44" s="14" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="D44" s="13"/>
     </row>
     <row r="45" customFormat="false" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="11" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="B45" s="11" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="C45" s="14" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="D45" s="13"/>
     </row>
     <row r="46" customFormat="false" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="11" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="B46" s="11" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="C46" s="14" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="D46" s="11" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="11" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="B47" s="11" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="C47" s="14" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="D47" s="11" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="11" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="B48" s="11" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="C48" s="14" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="D48" s="11" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="11" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="B49" s="11" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="C49" s="14" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="D49" s="11" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="11" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="B50" s="11" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="C50" s="14" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="D50" s="11" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="11" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="B51" s="11" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="C51" s="14" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="D51" s="11" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="11" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="B52" s="11" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
       <c r="C52" s="14" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="D52" s="13"/>
     </row>
     <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="11" t="s">
-        <v>195</v>
+        <v>197</v>
       </c>
       <c r="B53" s="11" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="C53" s="14" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="D53" s="13"/>
     </row>
     <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="11" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="B54" s="11" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="C54" s="14" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="D54" s="13"/>
     </row>
     <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="11" t="s">
-        <v>201</v>
+        <v>203</v>
       </c>
       <c r="B55" s="11" t="s">
-        <v>202</v>
+        <v>204</v>
       </c>
       <c r="C55" s="14" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
       <c r="D55" s="13"/>
     </row>
     <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="11" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="B56" s="11" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="C56" s="14" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="D56" s="13"/>
     </row>
     <row r="57" customFormat="false" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="11" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
       <c r="B57" s="11" t="s">
-        <v>208</v>
+        <v>210</v>
       </c>
       <c r="C57" s="14" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="D57" s="11" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="11" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
       <c r="B58" s="11" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="C58" s="14" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
       <c r="D58" s="13"/>
     </row>
     <row r="59" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="11" t="s">
-        <v>214</v>
+        <v>216</v>
       </c>
       <c r="B59" s="11" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
       <c r="C59" s="14" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="D59" s="13"/>
     </row>
     <row r="60" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="11" t="s">
-        <v>217</v>
+        <v>219</v>
       </c>
       <c r="B60" s="11" t="s">
-        <v>218</v>
+        <v>220</v>
       </c>
       <c r="C60" s="14" t="s">
-        <v>219</v>
+        <v>221</v>
       </c>
       <c r="D60" s="13"/>
     </row>
     <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="11" t="s">
-        <v>220</v>
+        <v>222</v>
       </c>
       <c r="B61" s="11" t="s">
-        <v>221</v>
+        <v>223</v>
       </c>
       <c r="C61" s="14" t="s">
-        <v>222</v>
+        <v>224</v>
       </c>
       <c r="D61" s="13"/>
     </row>
     <row r="62" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="11" t="s">
-        <v>223</v>
+        <v>225</v>
       </c>
       <c r="B62" s="11" t="s">
-        <v>224</v>
+        <v>226</v>
       </c>
       <c r="C62" s="14" t="s">
-        <v>225</v>
+        <v>227</v>
       </c>
       <c r="D62" s="13"/>
     </row>
     <row r="63" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="11" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
       <c r="B63" s="11" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="C63" s="14" t="s">
-        <v>228</v>
+        <v>230</v>
       </c>
       <c r="D63" s="13"/>
     </row>
     <row r="64" customFormat="false" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="11" t="s">
-        <v>229</v>
+        <v>231</v>
       </c>
       <c r="B64" s="11" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
       <c r="C64" s="14" t="s">
-        <v>231</v>
+        <v>233</v>
       </c>
       <c r="D64" s="13"/>
     </row>
     <row r="65" customFormat="false" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="11" t="s">
-        <v>232</v>
+        <v>234</v>
       </c>
       <c r="B65" s="11" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="C65" s="14" t="s">
-        <v>234</v>
+        <v>236</v>
       </c>
       <c r="D65" s="13"/>
     </row>
     <row r="66" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="11" t="s">
-        <v>235</v>
+        <v>237</v>
       </c>
       <c r="B66" s="11" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="C66" s="14" t="s">
-        <v>237</v>
+        <v>239</v>
       </c>
       <c r="D66" s="11" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="11" t="s">
-        <v>239</v>
+        <v>241</v>
       </c>
       <c r="B67" s="11" t="s">
-        <v>240</v>
+        <v>242</v>
       </c>
       <c r="C67" s="14" t="s">
-        <v>241</v>
+        <v>243</v>
       </c>
       <c r="D67" s="11" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="55.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="10" t="s">
-        <v>242</v>
+        <v>244</v>
       </c>
       <c r="B68" s="11" t="s">
-        <v>243</v>
+        <v>245</v>
       </c>
       <c r="C68" s="14" t="s">
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="D68" s="13"/>
     </row>
     <row r="69" customFormat="false" ht="55.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="11" t="s">
-        <v>245</v>
+        <v>247</v>
       </c>
       <c r="B69" s="11" t="s">
-        <v>246</v>
+        <v>248</v>
       </c>
       <c r="C69" s="14" t="s">
-        <v>247</v>
+        <v>249</v>
       </c>
       <c r="D69" s="13"/>
     </row>
     <row r="70" customFormat="false" ht="55.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="11" t="s">
-        <v>248</v>
+        <v>250</v>
       </c>
       <c r="B70" s="11" t="s">
-        <v>249</v>
+        <v>251</v>
       </c>
       <c r="C70" s="14" t="s">
-        <v>250</v>
+        <v>252</v>
       </c>
       <c r="D70" s="13"/>
     </row>
     <row r="71" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="11" t="s">
-        <v>251</v>
+        <v>253</v>
       </c>
       <c r="B71" s="11" t="s">
-        <v>252</v>
+        <v>254</v>
       </c>
       <c r="C71" s="14" t="s">
-        <v>253</v>
+        <v>255</v>
       </c>
       <c r="D71" s="13"/>
     </row>
     <row r="72" customFormat="false" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="11" t="s">
-        <v>254</v>
+        <v>256</v>
       </c>
       <c r="B72" s="11" t="s">
-        <v>255</v>
+        <v>257</v>
       </c>
       <c r="C72" s="14" t="s">
-        <v>256</v>
+        <v>258</v>
       </c>
       <c r="D72" s="11" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="42" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="11" t="s">
-        <v>257</v>
+        <v>259</v>
       </c>
       <c r="B73" s="11" t="s">
-        <v>258</v>
+        <v>260</v>
       </c>
       <c r="C73" s="14" t="s">
-        <v>259</v>
+        <v>261</v>
       </c>
       <c r="D73" s="11" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="11" t="s">
-        <v>260</v>
+        <v>262</v>
       </c>
       <c r="B74" s="11" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="C74" s="14" t="s">
-        <v>262</v>
+        <v>264</v>
       </c>
       <c r="D74" s="13"/>
     </row>
     <row r="75" customFormat="false" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="11" t="s">
-        <v>263</v>
+        <v>265</v>
       </c>
       <c r="B75" s="11" t="s">
-        <v>264</v>
+        <v>266</v>
       </c>
       <c r="C75" s="14" t="s">
-        <v>265</v>
+        <v>267</v>
       </c>
       <c r="D75" s="13"/>
     </row>
     <row r="76" customFormat="false" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="11" t="s">
-        <v>266</v>
+        <v>268</v>
       </c>
       <c r="B76" s="11" t="s">
-        <v>267</v>
+        <v>269</v>
       </c>
       <c r="C76" s="14" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
       <c r="D76" s="13"/>
     </row>
     <row r="77" customFormat="false" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="11" t="s">
-        <v>269</v>
+        <v>271</v>
       </c>
       <c r="B77" s="11" t="s">
-        <v>270</v>
+        <v>272</v>
       </c>
       <c r="C77" s="14" t="s">
-        <v>271</v>
+        <v>273</v>
       </c>
       <c r="D77" s="13"/>
     </row>
     <row r="78" customFormat="false" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="11" t="s">
-        <v>272</v>
+        <v>274</v>
       </c>
       <c r="B78" s="11" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="C78" s="14" t="s">
-        <v>274</v>
+        <v>276</v>
       </c>
       <c r="D78" s="13"/>
     </row>
     <row r="79" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="11" t="s">
-        <v>275</v>
+        <v>277</v>
       </c>
       <c r="B79" s="11" t="s">
-        <v>276</v>
+        <v>278</v>
       </c>
       <c r="C79" s="14" t="s">
-        <v>277</v>
+        <v>279</v>
       </c>
       <c r="D79" s="13"/>
     </row>
     <row r="80" customFormat="false" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="11" t="s">
-        <v>278</v>
+        <v>280</v>
       </c>
       <c r="B80" s="11" t="s">
-        <v>279</v>
+        <v>281</v>
       </c>
       <c r="C80" s="14" t="s">
-        <v>280</v>
+        <v>282</v>
       </c>
       <c r="D80" s="11" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="42" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="11" t="s">
-        <v>281</v>
+        <v>283</v>
       </c>
       <c r="B81" s="11" t="s">
-        <v>282</v>
+        <v>284</v>
       </c>
       <c r="C81" s="14" t="s">
-        <v>283</v>
+        <v>285</v>
       </c>
       <c r="D81" s="11" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="11" t="s">
-        <v>284</v>
+        <v>286</v>
       </c>
       <c r="B82" s="11" t="s">
-        <v>285</v>
+        <v>287</v>
       </c>
       <c r="C82" s="14" t="s">
-        <v>286</v>
+        <v>288</v>
       </c>
       <c r="D82" s="13"/>
     </row>
     <row r="83" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="11" t="s">
-        <v>287</v>
+        <v>289</v>
       </c>
       <c r="B83" s="11" t="s">
-        <v>288</v>
+        <v>290</v>
       </c>
       <c r="C83" s="14" t="s">
-        <v>287</v>
+        <v>289</v>
       </c>
       <c r="D83" s="13"/>
     </row>
     <row r="84" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="11" t="s">
-        <v>289</v>
+        <v>291</v>
       </c>
       <c r="B84" s="11" t="s">
-        <v>290</v>
+        <v>292</v>
       </c>
       <c r="C84" s="14" t="s">
-        <v>289</v>
+        <v>291</v>
       </c>
       <c r="D84" s="13"/>
     </row>
     <row r="85" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="11" t="s">
-        <v>291</v>
+        <v>293</v>
       </c>
       <c r="B85" s="11" t="s">
-        <v>292</v>
+        <v>294</v>
       </c>
       <c r="C85" s="14" t="s">
-        <v>291</v>
+        <v>293</v>
       </c>
       <c r="D85" s="13"/>
     </row>
     <row r="86" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="11" t="s">
-        <v>293</v>
+        <v>295</v>
       </c>
       <c r="B86" s="11" t="s">
-        <v>294</v>
+        <v>296</v>
       </c>
       <c r="C86" s="14" t="s">
-        <v>293</v>
+        <v>295</v>
       </c>
       <c r="D86" s="13"/>
     </row>
     <row r="87" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="11" t="s">
-        <v>295</v>
+        <v>297</v>
       </c>
       <c r="B87" s="11" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="C87" s="14" t="s">
-        <v>297</v>
+        <v>299</v>
       </c>
       <c r="D87" s="13"/>
     </row>
     <row r="88" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="11" t="s">
-        <v>298</v>
+        <v>300</v>
       </c>
       <c r="B88" s="11" t="s">
+        <v>301</v>
+      </c>
+      <c r="C88" s="14" t="s">
         <v>299</v>
       </c>
-      <c r="C88" s="14" t="s">
-        <v>297</v>
-      </c>
       <c r="D88" s="11" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="11" t="s">
-        <v>300</v>
+        <v>302</v>
       </c>
       <c r="B89" s="11" t="s">
-        <v>301</v>
+        <v>303</v>
       </c>
       <c r="C89" s="14" t="s">
-        <v>300</v>
+        <v>302</v>
       </c>
       <c r="D89" s="11" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="11" t="s">
-        <v>302</v>
+        <v>304</v>
       </c>
       <c r="B90" s="11" t="s">
-        <v>303</v>
+        <v>305</v>
       </c>
       <c r="C90" s="14" t="s">
-        <v>302</v>
+        <v>304</v>
       </c>
       <c r="D90" s="13"/>
     </row>
     <row r="91" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="11" t="s">
-        <v>304</v>
+        <v>306</v>
       </c>
       <c r="B91" s="11" t="s">
-        <v>305</v>
+        <v>307</v>
       </c>
       <c r="C91" s="14" t="s">
-        <v>304</v>
+        <v>306</v>
       </c>
       <c r="D91" s="13"/>
     </row>
     <row r="92" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="11" t="s">
-        <v>306</v>
+        <v>308</v>
       </c>
       <c r="B92" s="11" t="s">
-        <v>307</v>
+        <v>309</v>
       </c>
       <c r="C92" s="14" t="s">
-        <v>306</v>
+        <v>308</v>
       </c>
       <c r="D92" s="13"/>
     </row>
     <row r="93" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="11" t="s">
-        <v>308</v>
+        <v>310</v>
       </c>
       <c r="B93" s="11" t="s">
-        <v>309</v>
+        <v>311</v>
       </c>
       <c r="C93" s="14" t="s">
-        <v>308</v>
+        <v>310</v>
       </c>
       <c r="D93" s="13"/>
     </row>
     <row r="94" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="11" t="s">
-        <v>310</v>
+        <v>312</v>
       </c>
       <c r="B94" s="11" t="s">
-        <v>311</v>
+        <v>313</v>
       </c>
       <c r="C94" s="14" t="s">
-        <v>310</v>
+        <v>312</v>
       </c>
       <c r="D94" s="13"/>
     </row>
     <row r="95" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="11" t="s">
-        <v>312</v>
+        <v>314</v>
       </c>
       <c r="B95" s="11" t="s">
-        <v>313</v>
+        <v>315</v>
       </c>
       <c r="C95" s="14" t="s">
-        <v>312</v>
+        <v>314</v>
       </c>
       <c r="D95" s="13"/>
     </row>
     <row r="96" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="11" t="s">
-        <v>312</v>
+        <v>314</v>
       </c>
       <c r="B96" s="11" t="s">
+        <v>316</v>
+      </c>
+      <c r="C96" s="14" t="s">
         <v>314</v>
       </c>
-      <c r="C96" s="14" t="s">
-        <v>312</v>
-      </c>
       <c r="D96" s="11" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="11" t="s">
-        <v>315</v>
+        <v>317</v>
       </c>
       <c r="B97" s="11" t="s">
-        <v>316</v>
+        <v>318</v>
       </c>
       <c r="C97" s="14" t="s">
-        <v>315</v>
+        <v>317</v>
       </c>
       <c r="D97" s="11" t="s">
         <v>7</v>
@@ -2833,161 +2813,161 @@
     </row>
     <row r="98" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="11" t="s">
-        <v>317</v>
+        <v>319</v>
       </c>
       <c r="B98" s="11" t="s">
-        <v>318</v>
+        <v>320</v>
       </c>
       <c r="C98" s="14" t="s">
-        <v>317</v>
+        <v>319</v>
       </c>
       <c r="D98" s="13"/>
     </row>
     <row r="99" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="11" t="s">
-        <v>319</v>
+        <v>321</v>
       </c>
       <c r="B99" s="11" t="s">
-        <v>320</v>
+        <v>322</v>
       </c>
       <c r="C99" s="14" t="s">
-        <v>319</v>
+        <v>321</v>
       </c>
       <c r="D99" s="13"/>
     </row>
     <row r="100" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="11" t="s">
-        <v>321</v>
+        <v>323</v>
       </c>
       <c r="B100" s="11" t="s">
-        <v>322</v>
+        <v>324</v>
       </c>
       <c r="C100" s="14" t="s">
-        <v>321</v>
+        <v>323</v>
       </c>
       <c r="D100" s="13"/>
     </row>
     <row r="101" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="11" t="s">
-        <v>323</v>
+        <v>325</v>
       </c>
       <c r="B101" s="11" t="s">
-        <v>324</v>
+        <v>326</v>
       </c>
       <c r="C101" s="14" t="s">
-        <v>323</v>
+        <v>325</v>
       </c>
       <c r="D101" s="13"/>
     </row>
     <row r="102" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="11" t="s">
-        <v>325</v>
+        <v>327</v>
       </c>
       <c r="B102" s="11" t="s">
-        <v>326</v>
+        <v>328</v>
       </c>
       <c r="C102" s="14" t="s">
-        <v>325</v>
+        <v>327</v>
       </c>
       <c r="D102" s="13"/>
     </row>
     <row r="103" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A103" s="11" t="s">
-        <v>327</v>
+        <v>329</v>
       </c>
       <c r="B103" s="11" t="s">
-        <v>328</v>
+        <v>330</v>
       </c>
       <c r="C103" s="14" t="s">
-        <v>327</v>
+        <v>329</v>
       </c>
       <c r="D103" s="13"/>
     </row>
     <row r="104" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A104" s="10" t="s">
-        <v>327</v>
+        <v>329</v>
       </c>
       <c r="B104" s="11" t="s">
+        <v>331</v>
+      </c>
+      <c r="C104" s="14" t="s">
         <v>329</v>
       </c>
-      <c r="C104" s="14" t="s">
-        <v>327</v>
-      </c>
       <c r="D104" s="11" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
     </row>
     <row r="105" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A105" s="11" t="s">
-        <v>330</v>
+        <v>332</v>
       </c>
       <c r="B105" s="11" t="s">
-        <v>331</v>
+        <v>333</v>
       </c>
       <c r="C105" s="14" t="s">
-        <v>330</v>
+        <v>332</v>
       </c>
       <c r="D105" s="11" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
     </row>
     <row r="106" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A106" s="11" t="s">
-        <v>332</v>
+        <v>334</v>
       </c>
       <c r="B106" s="11" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
       <c r="C106" s="14" t="s">
-        <v>332</v>
+        <v>334</v>
       </c>
       <c r="D106" s="13"/>
     </row>
     <row r="107" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A107" s="11" t="s">
-        <v>334</v>
+        <v>336</v>
       </c>
       <c r="B107" s="11" t="s">
-        <v>335</v>
+        <v>337</v>
       </c>
       <c r="C107" s="14" t="s">
-        <v>334</v>
+        <v>336</v>
       </c>
       <c r="D107" s="13"/>
     </row>
     <row r="108" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A108" s="11" t="s">
-        <v>336</v>
+        <v>338</v>
       </c>
       <c r="B108" s="11" t="s">
-        <v>337</v>
+        <v>339</v>
       </c>
       <c r="C108" s="14" t="s">
-        <v>336</v>
+        <v>338</v>
       </c>
       <c r="D108" s="13"/>
     </row>
     <row r="109" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A109" s="11" t="s">
-        <v>338</v>
+        <v>340</v>
       </c>
       <c r="B109" s="11" t="s">
-        <v>339</v>
+        <v>341</v>
       </c>
       <c r="C109" s="14" t="s">
-        <v>340</v>
+        <v>342</v>
       </c>
       <c r="D109" s="13"/>
     </row>
     <row r="110" customFormat="false" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A110" s="10" t="s">
-        <v>341</v>
+        <v>343</v>
       </c>
       <c r="B110" s="11" t="s">
-        <v>342</v>
+        <v>344</v>
       </c>
       <c r="C110" s="14" t="s">
-        <v>343</v>
+        <v>345</v>
       </c>
       <c r="D110" s="13"/>
     </row>
@@ -3000,78 +2980,4 @@
     <oddFooter/>
   </headerFooter>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:E6"/>
-  <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F2" activeCellId="0" sqref="F2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="2" width="26.16"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="2" width="15.74"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="4" min="4" style="2" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="2" width="21.02"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="6" style="2" width="11.52"/>
-  </cols>
-  <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="3" t="s">
-        <v>344</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>345</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>346</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="15" t="s">
-        <v>44</v>
-      </c>
-      <c r="C2" s="16" t="s">
-        <v>347</v>
-      </c>
-      <c r="E2" s="16" t="s">
-        <v>348</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="17" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="17" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="17" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="17" t="s">
-        <v>99</v>
-      </c>
-    </row>
-  </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
-  </headerFooter>
-</worksheet>
 </file>
</xml_diff>